<commit_message>
Reran experiments with new Overview
</commit_message>
<xml_diff>
--- a/Evaluation/eval002/Classifcation Report.xlsx
+++ b/Evaluation/eval002/Classifcation Report.xlsx
@@ -400,13 +400,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9873417721518988</v>
+        <v>0.9506172839506173</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7722772277227723</v>
+        <v>0.7623762376237624</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8666666666666666</v>
+        <v>0.8461538461538463</v>
       </c>
       <c r="E2" t="n">
         <v>101</v>
@@ -419,13 +419,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8130081300813008</v>
+        <v>0.8016528925619835</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9900990099009901</v>
+        <v>0.9603960396039604</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8928571428571429</v>
+        <v>0.8738738738738738</v>
       </c>
       <c r="E3" t="n">
         <v>101</v>
@@ -438,16 +438,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8811881188118812</v>
+        <v>0.8613861386138614</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8811881188118812</v>
+        <v>0.8613861386138614</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8811881188118812</v>
+        <v>0.8613861386138614</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8811881188118812</v>
+        <v>0.8613861386138614</v>
       </c>
     </row>
     <row r="5">
@@ -457,13 +457,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9001749511165997</v>
+        <v>0.8761350882563004</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8811881188118812</v>
+        <v>0.8613861386138614</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8797619047619047</v>
+        <v>0.86001386001386</v>
       </c>
       <c r="E5" t="n">
         <v>202</v>
@@ -476,13 +476,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9001749511165998</v>
+        <v>0.8761350882563004</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8811881188118812</v>
+        <v>0.8613861386138614</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8797619047619047</v>
+        <v>0.86001386001386</v>
       </c>
       <c r="E6" t="n">
         <v>202</v>

</xml_diff>